<commit_message>
ok final for tonight
</commit_message>
<xml_diff>
--- a/WF/temp/products.xlsx
+++ b/WF/temp/products.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H60"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2043,6 +2043,326 @@
         </is>
       </c>
     </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>50</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Ceramic Pot - 8 inch</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Durable ceramic pot perfect for indoor plants.</t>
+        </is>
+      </c>
+      <c r="D51" t="n">
+        <v>50</v>
+      </c>
+      <c r="E51" t="n">
+        <v>15.99</v>
+      </c>
+      <c r="F51" t="n">
+        <v>10</v>
+      </c>
+      <c r="G51" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>51</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Mini Pot Planters - 10 pcs</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Set of 10 colorful mini planters for small plants.</t>
+        </is>
+      </c>
+      <c r="D52" t="n">
+        <v>100</v>
+      </c>
+      <c r="E52" t="n">
+        <v>12.5</v>
+      </c>
+      <c r="F52" t="n">
+        <v>8</v>
+      </c>
+      <c r="G52" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>52</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Terracotta Pot - 12 inch</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Classic terracotta pot for garden and patio use.</t>
+        </is>
+      </c>
+      <c r="D53" t="n">
+        <v>40</v>
+      </c>
+      <c r="E53" t="n">
+        <v>18.75</v>
+      </c>
+      <c r="F53" t="n">
+        <v>12</v>
+      </c>
+      <c r="G53" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>53</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Hanging Pot Set - 3 pcs</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Hanging pot set with metal chains for balconies.</t>
+        </is>
+      </c>
+      <c r="D54" t="n">
+        <v>30</v>
+      </c>
+      <c r="E54" t="n">
+        <v>22</v>
+      </c>
+      <c r="F54" t="n">
+        <v>15</v>
+      </c>
+      <c r="G54" t="b">
+        <v>1</v>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>54</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Glass Pot for Succulents</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Transparent glass pot ideal for succulent display.</t>
+        </is>
+      </c>
+      <c r="D55" t="n">
+        <v>60</v>
+      </c>
+      <c r="E55" t="n">
+        <v>14.99</v>
+      </c>
+      <c r="F55" t="n">
+        <v>9.5</v>
+      </c>
+      <c r="G55" t="b">
+        <v>1</v>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>55</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Large Outdoor Pot - 20 inch</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Large outdoor pot designed for trees and shrubs.</t>
+        </is>
+      </c>
+      <c r="D56" t="n">
+        <v>20</v>
+      </c>
+      <c r="E56" t="n">
+        <v>35</v>
+      </c>
+      <c r="F56" t="n">
+        <v>25</v>
+      </c>
+      <c r="G56" t="b">
+        <v>1</v>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>56</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Decorative Pot with Stand</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Decorative pot with wooden stand for living rooms.</t>
+        </is>
+      </c>
+      <c r="D57" t="n">
+        <v>25</v>
+      </c>
+      <c r="E57" t="n">
+        <v>29.99</v>
+      </c>
+      <c r="F57" t="n">
+        <v>20</v>
+      </c>
+      <c r="G57" t="b">
+        <v>1</v>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>57</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Plastic Pot - 5 inch</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Sturdy plastic pot suitable for various plants.</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>70</v>
+      </c>
+      <c r="E58" t="n">
+        <v>10</v>
+      </c>
+      <c r="F58" t="n">
+        <v>6.5</v>
+      </c>
+      <c r="G58" t="b">
+        <v>1</v>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="n">
+        <v>58</v>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Bamboo Pot - Eco Friendly</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Eco-friendly bamboo pot for sustainable gardening.</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>45</v>
+      </c>
+      <c r="E59" t="n">
+        <v>16.5</v>
+      </c>
+      <c r="F59" t="n">
+        <v>11</v>
+      </c>
+      <c r="G59" t="b">
+        <v>1</v>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="n">
+        <v>59</v>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Self-Watering Pot - 6 inch</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Self-watering pot to keep plants hydrated longer.</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>55</v>
+      </c>
+      <c r="E60" t="n">
+        <v>19.99</v>
+      </c>
+      <c r="F60" t="n">
+        <v>13</v>
+      </c>
+      <c r="G60" t="b">
+        <v>1</v>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>['All', 'Pots']</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>